<commit_message>
Commit avant changement sur Logit VNF
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="172">
   <si>
     <t>X1</t>
   </si>
@@ -527,82 +527,7 @@
     <t>0.796</t>
   </si>
   <si>
-    <t>0.975</t>
-  </si>
-  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>1.68</t>
-  </si>
-  <si>
-    <t>0.286</t>
-  </si>
-  <si>
-    <t>9.46e-08</t>
-  </si>
-  <si>
-    <t>0.393</t>
-  </si>
-  <si>
-    <t>1.78</t>
-  </si>
-  <si>
-    <t>2.07</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-  <si>
-    <t>7.94e-08</t>
-  </si>
-  <si>
-    <t>[0.93;1.021]</t>
-  </si>
-  <si>
-    <t>[0.64;4.362]</t>
-  </si>
-  <si>
-    <t>[0.087;0.913]</t>
-  </si>
-  <si>
-    <t>[NA;1.47480695333869e+108]</t>
-  </si>
-  <si>
-    <t>[0.017;3.861]</t>
-  </si>
-  <si>
-    <t>[0.384;9.079]</t>
-  </si>
-  <si>
-    <t>[0.159;51.398]</t>
-  </si>
-  <si>
-    <t>[0.069;2.261]</t>
-  </si>
-  <si>
-    <t>[NA;1.13324460320633e+205]</t>
-  </si>
-  <si>
-    <t>0.288</t>
-  </si>
-  <si>
-    <t>0.284</t>
-  </si>
-  <si>
-    <t>0.458</t>
-  </si>
-  <si>
-    <t>0.466</t>
-  </si>
-  <si>
-    <t>0.587</t>
-  </si>
-  <si>
-    <t>0.332</t>
-  </si>
-  <si>
-    <t>0.995</t>
   </si>
 </sst>
 </file>
@@ -716,10 +641,10 @@
         <v>171</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G3" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4">
@@ -736,13 +661,13 @@
         <v>134</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5">
@@ -759,13 +684,13 @@
         <v>135</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6">
@@ -782,13 +707,13 @@
         <v>136</v>
       </c>
       <c r="E6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7">
@@ -805,13 +730,13 @@
         <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8">
@@ -828,13 +753,13 @@
         <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9">
@@ -851,13 +776,13 @@
         <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10">
@@ -874,13 +799,13 @@
         <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11">
@@ -897,13 +822,13 @@
         <v>140</v>
       </c>
       <c r="E11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12">
@@ -920,13 +845,13 @@
         <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13">
@@ -943,13 +868,13 @@
         <v>142</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G13" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14">
@@ -966,13 +891,13 @@
         <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15">
@@ -989,13 +914,13 @@
         <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16">
@@ -1012,13 +937,13 @@
         <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17">
@@ -1035,13 +960,13 @@
         <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18">
@@ -1058,13 +983,13 @@
         <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19">
@@ -1081,13 +1006,13 @@
         <v>148</v>
       </c>
       <c r="E19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20">
@@ -1104,13 +1029,13 @@
         <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F20" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G20" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21">
@@ -1127,13 +1052,13 @@
         <v>149</v>
       </c>
       <c r="E21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F21" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G21" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22">
@@ -1150,13 +1075,13 @@
         <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F22" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G22" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23">
@@ -1173,13 +1098,13 @@
         <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="G23" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24">
@@ -1196,13 +1121,13 @@
         <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F24" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="G24" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25">
@@ -1219,13 +1144,13 @@
         <v>153</v>
       </c>
       <c r="E25" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F25" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="G25" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26">
@@ -1242,13 +1167,13 @@
         <v>154</v>
       </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F26" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="G26" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27">
@@ -1265,13 +1190,13 @@
         <v>155</v>
       </c>
       <c r="E27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28">
@@ -1288,13 +1213,13 @@
         <v>156</v>
       </c>
       <c r="E28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29">
@@ -1311,13 +1236,13 @@
         <v>157</v>
       </c>
       <c r="E29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30">
@@ -1334,13 +1259,13 @@
         <v>158</v>
       </c>
       <c r="E30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31">
@@ -1357,13 +1282,13 @@
         <v>159</v>
       </c>
       <c r="E31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32">
@@ -1380,13 +1305,13 @@
         <v>149</v>
       </c>
       <c r="E32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33">
@@ -1403,13 +1328,13 @@
         <v>160</v>
       </c>
       <c r="E33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34">
@@ -1426,13 +1351,13 @@
         <v>161</v>
       </c>
       <c r="E34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35">
@@ -1449,13 +1374,13 @@
         <v>162</v>
       </c>
       <c r="E35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36">
@@ -1472,13 +1397,13 @@
         <v>163</v>
       </c>
       <c r="E36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37">
@@ -1495,13 +1420,13 @@
         <v>164</v>
       </c>
       <c r="E37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38">
@@ -1518,13 +1443,13 @@
         <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39">
@@ -1541,13 +1466,13 @@
         <v>145</v>
       </c>
       <c r="E39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40">
@@ -1564,13 +1489,13 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41">
@@ -1587,13 +1512,13 @@
         <v>167</v>
       </c>
       <c r="E41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42">
@@ -1610,13 +1535,13 @@
         <v>168</v>
       </c>
       <c r="E42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43">
@@ -1633,13 +1558,13 @@
         <v>169</v>
       </c>
       <c r="E43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44">
@@ -1656,13 +1581,13 @@
         <v>170</v>
       </c>
       <c r="E44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>